<commit_message>
Linear mixed effect model implemented in code
tilt angles calculated and updated in experimental data file
</commit_message>
<xml_diff>
--- a/Data/experiment_data_all-210105210502.xlsx
+++ b/Data/experiment_data_all-210105210502.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adwait\Desktop\MPIP\Work\20210105 effect of contact all\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Documents\paper-underwater_adhesion\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="settings" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$CA$485</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$CD$485</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14700" uniqueCount="4672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14703" uniqueCount="4675">
   <si>
     <t>index</t>
   </si>
@@ -14039,12 +14039,21 @@
   </si>
   <si>
     <t>Substrate equal to Glass AND Contact Type equal to Dry AND Data OK? equal to Yes None</t>
+  </si>
+  <si>
+    <t>Top angle</t>
+  </si>
+  <si>
+    <t>Bottom angle</t>
+  </si>
+  <si>
+    <t>Tilt angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -14073,7 +14082,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -14096,16 +14105,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14410,15 +14433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA485"/>
+  <dimension ref="A1:CD485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14653,8 +14676,17 @@
       <c r="CA1" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="CB1" s="3" t="s">
+        <v>4672</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>4673</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>4674</v>
+      </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -14806,7 +14838,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -14958,7 +14990,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -15110,7 +15142,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -15262,7 +15294,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -15414,7 +15446,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -15566,7 +15598,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -15718,7 +15750,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -15870,7 +15902,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="10" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -16025,7 +16057,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -16180,7 +16212,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -16335,7 +16367,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -16490,7 +16522,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -16645,7 +16677,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -16800,7 +16832,7 @@
         <v>4026</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -51727,7 +51759,7 @@
         <v>108.7024457299522</v>
       </c>
     </row>
-    <row r="225" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -51918,7 +51950,7 @@
         <v>83.685990182912064</v>
       </c>
     </row>
-    <row r="226" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -52106,7 +52138,7 @@
         <v>917.11749718094677</v>
       </c>
     </row>
-    <row r="227" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -52294,7 +52326,7 @@
         <v>919.53689162680041</v>
       </c>
     </row>
-    <row r="228" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -52482,7 +52514,7 @@
         <v>859.33114840355529</v>
       </c>
     </row>
-    <row r="229" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -52670,7 +52702,7 @@
         <v>977.5846748830977</v>
       </c>
     </row>
-    <row r="230" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -52858,7 +52890,7 @@
         <v>838.02062569231396</v>
       </c>
     </row>
-    <row r="231" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -53051,8 +53083,18 @@
       <c r="CA231">
         <v>767.07950879532746</v>
       </c>
+      <c r="CB231">
+        <v>14.57</v>
+      </c>
+      <c r="CC231">
+        <v>14.04</v>
+      </c>
+      <c r="CD231">
+        <f t="shared" ref="CD231:CD235" si="0">(CB231+CC231)/2</f>
+        <v>14.305</v>
+      </c>
     </row>
-    <row r="232" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -53245,8 +53287,18 @@
       <c r="CA232">
         <v>722.93021120705032</v>
       </c>
+      <c r="CB232">
+        <v>13.41</v>
+      </c>
+      <c r="CC232">
+        <v>14.44</v>
+      </c>
+      <c r="CD232">
+        <f t="shared" si="0"/>
+        <v>13.925000000000001</v>
+      </c>
     </row>
-    <row r="233" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -53439,8 +53491,18 @@
       <c r="CA233">
         <v>684.40213338388548</v>
       </c>
+      <c r="CB233">
+        <v>13.83</v>
+      </c>
+      <c r="CC233">
+        <v>16.82</v>
+      </c>
+      <c r="CD233">
+        <f t="shared" si="0"/>
+        <v>15.324999999999999</v>
+      </c>
     </row>
-    <row r="234" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -53633,8 +53695,18 @@
       <c r="CA234">
         <v>659.24698842352529</v>
       </c>
+      <c r="CB234">
+        <v>14.24</v>
+      </c>
+      <c r="CC234">
+        <v>15.77</v>
+      </c>
+      <c r="CD234">
+        <f t="shared" si="0"/>
+        <v>15.004999999999999</v>
+      </c>
     </row>
-    <row r="235" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -53827,8 +53899,18 @@
       <c r="CA235">
         <v>568.67908437243977</v>
       </c>
+      <c r="CB235">
+        <v>15.11</v>
+      </c>
+      <c r="CC235">
+        <v>14.88</v>
+      </c>
+      <c r="CD235">
+        <f t="shared" si="0"/>
+        <v>14.995000000000001</v>
+      </c>
     </row>
-    <row r="236" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -54016,7 +54098,7 @@
         <v>481.78069497606162</v>
       </c>
     </row>
-    <row r="237" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -54204,7 +54286,7 @@
         <v>611.40445257615579</v>
       </c>
     </row>
-    <row r="238" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -54392,7 +54474,7 @@
         <v>528.10700352771039</v>
       </c>
     </row>
-    <row r="239" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -54580,7 +54662,7 @@
         <v>571.48396080921509</v>
       </c>
     </row>
-    <row r="240" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -54768,7 +54850,7 @@
         <v>529.70486512684329</v>
       </c>
     </row>
-    <row r="241" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -54961,8 +55043,17 @@
       <c r="CA241">
         <v>467.47992589055548</v>
       </c>
+      <c r="CB241">
+        <v>23.36</v>
+      </c>
+      <c r="CC241">
+        <v>21.57</v>
+      </c>
+      <c r="CD241">
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="242" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -55155,8 +55246,17 @@
       <c r="CA242">
         <v>730.31569888998229</v>
       </c>
+      <c r="CB242">
+        <v>23.36</v>
+      </c>
+      <c r="CC242">
+        <v>21.57</v>
+      </c>
+      <c r="CD242">
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="243" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -55349,8 +55449,17 @@
       <c r="CA243">
         <v>675.24720292278823</v>
       </c>
+      <c r="CB243">
+        <v>23.36</v>
+      </c>
+      <c r="CC243">
+        <v>21.57</v>
+      </c>
+      <c r="CD243">
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="244" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -55543,8 +55652,17 @@
       <c r="CA244">
         <v>723.5064756132648</v>
       </c>
+      <c r="CB244">
+        <v>23.36</v>
+      </c>
+      <c r="CC244">
+        <v>21.57</v>
+      </c>
+      <c r="CD244">
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="245" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -55737,8 +55855,17 @@
       <c r="CA245">
         <v>711.25872653285023</v>
       </c>
+      <c r="CB245">
+        <v>23.36</v>
+      </c>
+      <c r="CC245">
+        <v>21.57</v>
+      </c>
+      <c r="CD245">
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="246" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -55926,7 +56053,7 @@
         <v>1343.200376043859</v>
       </c>
     </row>
-    <row r="247" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -56114,7 +56241,7 @@
         <v>1454.7244555528241</v>
       </c>
     </row>
-    <row r="248" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -56302,7 +56429,7 @@
         <v>1149.321382771112</v>
       </c>
     </row>
-    <row r="249" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -56490,7 +56617,7 @@
         <v>765.81556492123661</v>
       </c>
     </row>
-    <row r="250" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -56678,7 +56805,7 @@
         <v>420.57081007874621</v>
       </c>
     </row>
-    <row r="251" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -56871,8 +56998,17 @@
       <c r="CA251">
         <v>537.60841343064749</v>
       </c>
+      <c r="CB251">
+        <v>16.5</v>
+      </c>
+      <c r="CC251">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="CD251">
+        <v>16.844999999999999</v>
+      </c>
     </row>
-    <row r="252" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -57065,8 +57201,17 @@
       <c r="CA252">
         <v>536.63920254670757</v>
       </c>
+      <c r="CB252">
+        <v>16.5</v>
+      </c>
+      <c r="CC252">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="CD252">
+        <v>16.844999999999999</v>
+      </c>
     </row>
-    <row r="253" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -57259,8 +57404,17 @@
       <c r="CA253">
         <v>424.24799463448198</v>
       </c>
+      <c r="CB253">
+        <v>16.5</v>
+      </c>
+      <c r="CC253">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="CD253">
+        <v>16.844999999999999</v>
+      </c>
     </row>
-    <row r="254" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -57453,8 +57607,17 @@
       <c r="CA254">
         <v>478.87110760628372</v>
       </c>
+      <c r="CB254">
+        <v>16.5</v>
+      </c>
+      <c r="CC254">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="CD254">
+        <v>16.844999999999999</v>
+      </c>
     </row>
-    <row r="255" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -57647,8 +57810,17 @@
       <c r="CA255">
         <v>566.0471849161803</v>
       </c>
+      <c r="CB255">
+        <v>16.5</v>
+      </c>
+      <c r="CC255">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="CD255">
+        <v>16.844999999999999</v>
+      </c>
     </row>
-    <row r="256" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -57836,7 +58008,7 @@
         <v>1289.906154033963</v>
       </c>
     </row>
-    <row r="257" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -58024,7 +58196,7 @@
         <v>1015.713029324868</v>
       </c>
     </row>
-    <row r="258" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -58212,7 +58384,7 @@
         <v>985.20399048833042</v>
       </c>
     </row>
-    <row r="259" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -58400,7 +58572,7 @@
         <v>940.79557248985247</v>
       </c>
     </row>
-    <row r="260" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -58588,7 +58760,7 @@
         <v>527.18171299576318</v>
       </c>
     </row>
-    <row r="261" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -58781,8 +58953,17 @@
       <c r="CA261">
         <v>1787.933525150954</v>
       </c>
+      <c r="CB261">
+        <v>8.93</v>
+      </c>
+      <c r="CC261">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="CD261">
+        <v>9.0249999999999986</v>
+      </c>
     </row>
-    <row r="262" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -58975,8 +59156,17 @@
       <c r="CA262">
         <v>1949.769592903255</v>
       </c>
+      <c r="CB262">
+        <v>8.93</v>
+      </c>
+      <c r="CC262">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="CD262">
+        <v>9.0249999999999986</v>
+      </c>
     </row>
-    <row r="263" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -59169,8 +59359,17 @@
       <c r="CA263">
         <v>1865.6569670967549</v>
       </c>
+      <c r="CB263">
+        <v>8.93</v>
+      </c>
+      <c r="CC263">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="CD263">
+        <v>9.0249999999999986</v>
+      </c>
     </row>
-    <row r="264" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -59363,8 +59562,17 @@
       <c r="CA264">
         <v>1998.1798071403971</v>
       </c>
+      <c r="CB264">
+        <v>8.93</v>
+      </c>
+      <c r="CC264">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="CD264">
+        <v>9.0249999999999986</v>
+      </c>
     </row>
-    <row r="265" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -59557,8 +59765,17 @@
       <c r="CA265">
         <v>1053.6249367122509</v>
       </c>
+      <c r="CB265">
+        <v>8.93</v>
+      </c>
+      <c r="CC265">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="CD265">
+        <v>9.0249999999999986</v>
+      </c>
     </row>
-    <row r="266" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -59746,7 +59963,7 @@
         <v>437.93252293686959</v>
       </c>
     </row>
-    <row r="267" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -59934,7 +60151,7 @@
         <v>365.81774968804092</v>
       </c>
     </row>
-    <row r="268" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -60122,7 +60339,7 @@
         <v>384.62799335950302</v>
       </c>
     </row>
-    <row r="269" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -60310,7 +60527,7 @@
         <v>351.16546467769342</v>
       </c>
     </row>
-    <row r="270" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -60498,7 +60715,7 @@
         <v>308.05435814288029</v>
       </c>
     </row>
-    <row r="271" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -60691,8 +60908,17 @@
       <c r="CA271">
         <v>601.02743904367162</v>
       </c>
+      <c r="CB271">
+        <v>20.7</v>
+      </c>
+      <c r="CC271">
+        <v>18.95</v>
+      </c>
+      <c r="CD271">
+        <v>19.824999999999999</v>
+      </c>
     </row>
-    <row r="272" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -60885,8 +61111,17 @@
       <c r="CA272">
         <v>886.76382702821638</v>
       </c>
+      <c r="CB272">
+        <v>20.7</v>
+      </c>
+      <c r="CC272">
+        <v>18.95</v>
+      </c>
+      <c r="CD272">
+        <v>19.824999999999999</v>
+      </c>
     </row>
-    <row r="273" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -61079,8 +61314,17 @@
       <c r="CA273">
         <v>971.29103721488036</v>
       </c>
+      <c r="CB273">
+        <v>20.7</v>
+      </c>
+      <c r="CC273">
+        <v>18.95</v>
+      </c>
+      <c r="CD273">
+        <v>19.824999999999999</v>
+      </c>
     </row>
-    <row r="274" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -61273,8 +61517,17 @@
       <c r="CA274">
         <v>1089.7020631576411</v>
       </c>
+      <c r="CB274">
+        <v>20.7</v>
+      </c>
+      <c r="CC274">
+        <v>18.95</v>
+      </c>
+      <c r="CD274">
+        <v>19.824999999999999</v>
+      </c>
     </row>
-    <row r="275" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -61467,8 +61720,17 @@
       <c r="CA275">
         <v>1133.2557287526879</v>
       </c>
+      <c r="CB275">
+        <v>20.7</v>
+      </c>
+      <c r="CC275">
+        <v>18.95</v>
+      </c>
+      <c r="CD275">
+        <v>19.824999999999999</v>
+      </c>
     </row>
-    <row r="276" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -61656,7 +61918,7 @@
         <v>799.71807044708464</v>
       </c>
     </row>
-    <row r="277" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -61844,7 +62106,7 @@
         <v>729.3079621636092</v>
       </c>
     </row>
-    <row r="278" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -62032,7 +62294,7 @@
         <v>781.18461269836644</v>
       </c>
     </row>
-    <row r="279" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -62220,7 +62482,7 @@
         <v>541.80357143173069</v>
       </c>
     </row>
-    <row r="280" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -62408,7 +62670,7 @@
         <v>577.05681857433422</v>
       </c>
     </row>
-    <row r="281" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -62598,8 +62860,17 @@
       <c r="CA281">
         <v>318.85695733048709</v>
       </c>
+      <c r="CB281">
+        <v>16.32</v>
+      </c>
+      <c r="CC281">
+        <v>15.08</v>
+      </c>
+      <c r="CD281">
+        <v>15.7</v>
+      </c>
     </row>
-    <row r="282" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -62789,8 +63060,17 @@
       <c r="CA282">
         <v>319.828262413223</v>
       </c>
+      <c r="CB282">
+        <v>16.32</v>
+      </c>
+      <c r="CC282">
+        <v>15.08</v>
+      </c>
+      <c r="CD282">
+        <v>15.7</v>
+      </c>
     </row>
-    <row r="283" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -62980,8 +63260,17 @@
       <c r="CA283">
         <v>554.57637873420936</v>
       </c>
+      <c r="CB283">
+        <v>16.32</v>
+      </c>
+      <c r="CC283">
+        <v>15.08</v>
+      </c>
+      <c r="CD283">
+        <v>15.7</v>
+      </c>
     </row>
-    <row r="284" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -63171,8 +63460,17 @@
       <c r="CA284">
         <v>431.37839526479729</v>
       </c>
+      <c r="CB284">
+        <v>16.32</v>
+      </c>
+      <c r="CC284">
+        <v>15.08</v>
+      </c>
+      <c r="CD284">
+        <v>15.7</v>
+      </c>
     </row>
-    <row r="285" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -63362,8 +63660,17 @@
       <c r="CA285">
         <v>542.59768476300269</v>
       </c>
+      <c r="CB285">
+        <v>16.32</v>
+      </c>
+      <c r="CC285">
+        <v>15.08</v>
+      </c>
+      <c r="CD285">
+        <v>15.7</v>
+      </c>
     </row>
-    <row r="286" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -63550,8 +63857,17 @@
       <c r="CA286">
         <v>700.09267527073439</v>
       </c>
+      <c r="CB286">
+        <v>7.71</v>
+      </c>
+      <c r="CC286">
+        <v>9.6</v>
+      </c>
+      <c r="CD286">
+        <v>8.6549999999999994</v>
+      </c>
     </row>
-    <row r="287" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -63738,8 +64054,17 @@
       <c r="CA287">
         <v>1000.658443461927</v>
       </c>
+      <c r="CB287">
+        <v>7.71</v>
+      </c>
+      <c r="CC287">
+        <v>9.6</v>
+      </c>
+      <c r="CD287">
+        <v>8.6549999999999994</v>
+      </c>
     </row>
-    <row r="288" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -63926,8 +64251,17 @@
       <c r="CA288">
         <v>735.82673729258556</v>
       </c>
+      <c r="CB288">
+        <v>7.71</v>
+      </c>
+      <c r="CC288">
+        <v>9.6</v>
+      </c>
+      <c r="CD288">
+        <v>8.6549999999999994</v>
+      </c>
     </row>
-    <row r="289" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -64114,8 +64448,17 @@
       <c r="CA289">
         <v>706.71949110659443</v>
       </c>
+      <c r="CB289">
+        <v>7.71</v>
+      </c>
+      <c r="CC289">
+        <v>9.6</v>
+      </c>
+      <c r="CD289">
+        <v>8.6549999999999994</v>
+      </c>
     </row>
-    <row r="290" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -64302,8 +64645,17 @@
       <c r="CA290">
         <v>419.70596087398019</v>
       </c>
+      <c r="CB290">
+        <v>7.71</v>
+      </c>
+      <c r="CC290">
+        <v>9.6</v>
+      </c>
+      <c r="CD290">
+        <v>8.6549999999999994</v>
+      </c>
     </row>
-    <row r="291" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -64493,8 +64845,17 @@
       <c r="CA291">
         <v>290.47434177797783</v>
       </c>
+      <c r="CB291">
+        <v>0</v>
+      </c>
+      <c r="CC291">
+        <v>0</v>
+      </c>
+      <c r="CD291">
+        <v>0</v>
+      </c>
     </row>
-    <row r="292" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -64684,8 +65045,17 @@
       <c r="CA292">
         <v>279.10372344362349</v>
       </c>
+      <c r="CB292">
+        <v>0</v>
+      </c>
+      <c r="CC292">
+        <v>0</v>
+      </c>
+      <c r="CD292">
+        <v>0</v>
+      </c>
     </row>
-    <row r="293" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -64875,8 +65245,17 @@
       <c r="CA293">
         <v>242.35230195234359</v>
       </c>
+      <c r="CB293">
+        <v>0</v>
+      </c>
+      <c r="CC293">
+        <v>0</v>
+      </c>
+      <c r="CD293">
+        <v>0</v>
+      </c>
     </row>
-    <row r="294" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -65066,8 +65445,17 @@
       <c r="CA294">
         <v>213.74370526762141</v>
       </c>
+      <c r="CB294">
+        <v>0</v>
+      </c>
+      <c r="CC294">
+        <v>0</v>
+      </c>
+      <c r="CD294">
+        <v>0</v>
+      </c>
     </row>
-    <row r="295" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -65257,8 +65645,17 @@
       <c r="CA295">
         <v>216.85032073742519</v>
       </c>
+      <c r="CB295">
+        <v>0</v>
+      </c>
+      <c r="CC295">
+        <v>0</v>
+      </c>
+      <c r="CD295">
+        <v>0</v>
+      </c>
     </row>
-    <row r="296" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -65446,7 +65843,7 @@
         <v>293.72575860313327</v>
       </c>
     </row>
-    <row r="297" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -65634,7 +66031,7 @@
         <v>281.85571435362289</v>
       </c>
     </row>
-    <row r="298" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -65822,7 +66219,7 @@
         <v>281.2016697951932</v>
       </c>
     </row>
-    <row r="299" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -66010,7 +66407,7 @@
         <v>266.44124465372772</v>
       </c>
     </row>
-    <row r="300" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -66198,7 +66595,7 @@
         <v>285.70925007913218</v>
       </c>
     </row>
-    <row r="301" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -66388,8 +66785,17 @@
       <c r="CA301">
         <v>420.83724898433678</v>
       </c>
+      <c r="CB301">
+        <v>20.5</v>
+      </c>
+      <c r="CC301">
+        <v>20.22</v>
+      </c>
+      <c r="CD301">
+        <v>20.36</v>
+      </c>
     </row>
-    <row r="302" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -66579,8 +66985,17 @@
       <c r="CA302">
         <v>464.90007005519828</v>
       </c>
+      <c r="CB302">
+        <v>20.5</v>
+      </c>
+      <c r="CC302">
+        <v>20.22</v>
+      </c>
+      <c r="CD302">
+        <v>20.36</v>
+      </c>
     </row>
-    <row r="303" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -66770,8 +67185,17 @@
       <c r="CA303">
         <v>494.22579277482367</v>
       </c>
+      <c r="CB303">
+        <v>20.5</v>
+      </c>
+      <c r="CC303">
+        <v>20.22</v>
+      </c>
+      <c r="CD303">
+        <v>20.36</v>
+      </c>
     </row>
-    <row r="304" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -66961,8 +67385,17 @@
       <c r="CA304">
         <v>490.69363176167508</v>
       </c>
+      <c r="CB304">
+        <v>20.5</v>
+      </c>
+      <c r="CC304">
+        <v>20.22</v>
+      </c>
+      <c r="CD304">
+        <v>20.36</v>
+      </c>
     </row>
-    <row r="305" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -67152,8 +67585,17 @@
       <c r="CA305">
         <v>959.35768477736156</v>
       </c>
+      <c r="CB305">
+        <v>20.5</v>
+      </c>
+      <c r="CC305">
+        <v>20.22</v>
+      </c>
+      <c r="CD305">
+        <v>20.36</v>
+      </c>
     </row>
-    <row r="306" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -67340,8 +67782,17 @@
       <c r="CA306">
         <v>1384.253269891906</v>
       </c>
+      <c r="CB306">
+        <v>10.38</v>
+      </c>
+      <c r="CC306">
+        <v>10.38</v>
+      </c>
+      <c r="CD306">
+        <v>10.38</v>
+      </c>
     </row>
-    <row r="307" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -67528,8 +67979,17 @@
       <c r="CA307">
         <v>1332.8930396436799</v>
       </c>
+      <c r="CB307">
+        <v>10.38</v>
+      </c>
+      <c r="CC307">
+        <v>10.38</v>
+      </c>
+      <c r="CD307">
+        <v>10.38</v>
+      </c>
     </row>
-    <row r="308" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -67716,8 +68176,17 @@
       <c r="CA308">
         <v>1009.77198568889</v>
       </c>
+      <c r="CB308">
+        <v>10.38</v>
+      </c>
+      <c r="CC308">
+        <v>10.38</v>
+      </c>
+      <c r="CD308">
+        <v>10.38</v>
+      </c>
     </row>
-    <row r="309" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -67904,8 +68373,17 @@
       <c r="CA309">
         <v>1090.3925671675941</v>
       </c>
+      <c r="CB309">
+        <v>10.38</v>
+      </c>
+      <c r="CC309">
+        <v>10.38</v>
+      </c>
+      <c r="CD309">
+        <v>10.38</v>
+      </c>
     </row>
-    <row r="310" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -68092,8 +68570,17 @@
       <c r="CA310">
         <v>1274.1602045442171</v>
       </c>
+      <c r="CB310">
+        <v>10.38</v>
+      </c>
+      <c r="CC310">
+        <v>10.38</v>
+      </c>
+      <c r="CD310">
+        <v>10.38</v>
+      </c>
     </row>
-    <row r="311" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -68283,8 +68770,17 @@
       <c r="CA311">
         <v>158.6187774403256</v>
       </c>
+      <c r="CB311">
+        <v>0</v>
+      </c>
+      <c r="CC311">
+        <v>0</v>
+      </c>
+      <c r="CD311">
+        <v>0</v>
+      </c>
     </row>
-    <row r="312" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -68474,8 +68970,17 @@
       <c r="CA312">
         <v>84.705896556930369</v>
       </c>
+      <c r="CB312">
+        <v>0</v>
+      </c>
+      <c r="CC312">
+        <v>0</v>
+      </c>
+      <c r="CD312">
+        <v>0</v>
+      </c>
     </row>
-    <row r="313" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -68665,8 +69170,17 @@
       <c r="CA313">
         <v>89.108798460750222</v>
       </c>
+      <c r="CB313">
+        <v>0</v>
+      </c>
+      <c r="CC313">
+        <v>0</v>
+      </c>
+      <c r="CD313">
+        <v>0</v>
+      </c>
     </row>
-    <row r="314" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -68856,8 +69370,17 @@
       <c r="CA314">
         <v>79.4672231194604</v>
       </c>
+      <c r="CB314">
+        <v>0</v>
+      </c>
+      <c r="CC314">
+        <v>0</v>
+      </c>
+      <c r="CD314">
+        <v>0</v>
+      </c>
     </row>
-    <row r="315" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -69047,8 +69570,17 @@
       <c r="CA315">
         <v>85.560033159097657</v>
       </c>
+      <c r="CB315">
+        <v>0</v>
+      </c>
+      <c r="CC315">
+        <v>0</v>
+      </c>
+      <c r="CD315">
+        <v>0</v>
+      </c>
     </row>
-    <row r="316" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -69236,7 +69768,7 @@
         <v>535.26350158496496</v>
       </c>
     </row>
-    <row r="317" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -69424,7 +69956,7 @@
         <v>580.933555513187</v>
       </c>
     </row>
-    <row r="318" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -69612,7 +70144,7 @@
         <v>574.86893555440338</v>
       </c>
     </row>
-    <row r="319" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -69800,7 +70332,7 @@
         <v>557.65812799338062</v>
       </c>
     </row>
-    <row r="320" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -69988,7 +70520,7 @@
         <v>543.29879902707751</v>
       </c>
     </row>
-    <row r="321" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -70178,8 +70710,17 @@
       <c r="CA321">
         <v>581.86218315720771</v>
       </c>
+      <c r="CB321">
+        <v>25.52</v>
+      </c>
+      <c r="CC321">
+        <v>26.16</v>
+      </c>
+      <c r="CD321">
+        <v>25.84</v>
+      </c>
     </row>
-    <row r="322" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -70369,8 +70910,17 @@
       <c r="CA322">
         <v>597.56342975672123</v>
       </c>
+      <c r="CB322">
+        <v>25.52</v>
+      </c>
+      <c r="CC322">
+        <v>26.16</v>
+      </c>
+      <c r="CD322">
+        <v>25.84</v>
+      </c>
     </row>
-    <row r="323" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -70560,8 +71110,17 @@
       <c r="CA323">
         <v>612.02431837126642</v>
       </c>
+      <c r="CB323">
+        <v>25.52</v>
+      </c>
+      <c r="CC323">
+        <v>26.16</v>
+      </c>
+      <c r="CD323">
+        <v>25.84</v>
+      </c>
     </row>
-    <row r="324" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -70751,8 +71310,17 @@
       <c r="CA324">
         <v>558.55894532181037</v>
       </c>
+      <c r="CB324">
+        <v>25.52</v>
+      </c>
+      <c r="CC324">
+        <v>26.16</v>
+      </c>
+      <c r="CD324">
+        <v>25.84</v>
+      </c>
     </row>
-    <row r="325" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -70942,8 +71510,17 @@
       <c r="CA325">
         <v>668.93887187557038</v>
       </c>
+      <c r="CB325">
+        <v>25.52</v>
+      </c>
+      <c r="CC325">
+        <v>26.16</v>
+      </c>
+      <c r="CD325">
+        <v>25.84</v>
+      </c>
     </row>
-    <row r="326" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -71133,8 +71710,18 @@
       <c r="CA326">
         <v>656.93655317247078</v>
       </c>
+      <c r="CB326">
+        <v>18.03</v>
+      </c>
+      <c r="CC326">
+        <v>20.7</v>
+      </c>
+      <c r="CD326">
+        <f t="shared" ref="CD326:CD360" si="1">(CB326+CC326)/2</f>
+        <v>19.365000000000002</v>
+      </c>
     </row>
-    <row r="327" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -71324,8 +71911,18 @@
       <c r="CA327">
         <v>622.57536094935995</v>
       </c>
+      <c r="CB327">
+        <v>19.63</v>
+      </c>
+      <c r="CC327">
+        <v>21.01</v>
+      </c>
+      <c r="CD327">
+        <f t="shared" si="1"/>
+        <v>20.32</v>
+      </c>
     </row>
-    <row r="328" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -71515,8 +72112,18 @@
       <c r="CA328">
         <v>511.32360546614058</v>
       </c>
+      <c r="CB328">
+        <v>19.23</v>
+      </c>
+      <c r="CC328">
+        <v>19.88</v>
+      </c>
+      <c r="CD328">
+        <f t="shared" si="1"/>
+        <v>19.555</v>
+      </c>
     </row>
-    <row r="329" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -71706,8 +72313,18 @@
       <c r="CA329">
         <v>530.98226062532149</v>
       </c>
+      <c r="CB329">
+        <v>20.27</v>
+      </c>
+      <c r="CC329">
+        <v>20.37</v>
+      </c>
+      <c r="CD329">
+        <f t="shared" si="1"/>
+        <v>20.32</v>
+      </c>
     </row>
-    <row r="330" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -71897,8 +72514,18 @@
       <c r="CA330">
         <v>714.6751842211138</v>
       </c>
+      <c r="CB330">
+        <v>19.77</v>
+      </c>
+      <c r="CC330">
+        <v>19.37</v>
+      </c>
+      <c r="CD330">
+        <f t="shared" si="1"/>
+        <v>19.57</v>
+      </c>
     </row>
-    <row r="331" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -72091,8 +72718,18 @@
       <c r="CA331">
         <v>420.77892210495162</v>
       </c>
+      <c r="CB331">
+        <v>17.61</v>
+      </c>
+      <c r="CC331">
+        <v>20.41</v>
+      </c>
+      <c r="CD331">
+        <f t="shared" si="1"/>
+        <v>19.009999999999998</v>
+      </c>
     </row>
-    <row r="332" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -72285,8 +72922,18 @@
       <c r="CA332">
         <v>496.71146086613089</v>
       </c>
+      <c r="CB332">
+        <v>17.5</v>
+      </c>
+      <c r="CC332">
+        <v>18.97</v>
+      </c>
+      <c r="CD332">
+        <f t="shared" si="1"/>
+        <v>18.234999999999999</v>
+      </c>
     </row>
-    <row r="333" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -72479,8 +73126,18 @@
       <c r="CA333">
         <v>563.55921897743792</v>
       </c>
+      <c r="CB333">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="CC333">
+        <v>18.829999999999998</v>
+      </c>
+      <c r="CD333">
+        <f t="shared" si="1"/>
+        <v>19.32</v>
+      </c>
     </row>
-    <row r="334" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -72673,8 +73330,18 @@
       <c r="CA334">
         <v>606.09753162976176</v>
       </c>
+      <c r="CB334">
+        <v>18.43</v>
+      </c>
+      <c r="CC334">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="CD334">
+        <f t="shared" si="1"/>
+        <v>18.754999999999999</v>
+      </c>
     </row>
-    <row r="335" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -72867,8 +73534,18 @@
       <c r="CA335">
         <v>624.1168145788979</v>
       </c>
+      <c r="CB335">
+        <v>19.98</v>
+      </c>
+      <c r="CC335">
+        <v>20.22</v>
+      </c>
+      <c r="CD335">
+        <f t="shared" si="1"/>
+        <v>20.100000000000001</v>
+      </c>
     </row>
-    <row r="336" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -73055,8 +73732,18 @@
       <c r="CA336">
         <v>504.68819837227329</v>
       </c>
+      <c r="CB336">
+        <v>23.68</v>
+      </c>
+      <c r="CC336">
+        <v>28.19</v>
+      </c>
+      <c r="CD336">
+        <f t="shared" si="1"/>
+        <v>25.935000000000002</v>
+      </c>
     </row>
-    <row r="337" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -73243,8 +73930,18 @@
       <c r="CA337">
         <v>439.2477564187738</v>
       </c>
+      <c r="CB337">
+        <v>24.81</v>
+      </c>
+      <c r="CC337">
+        <v>29.19</v>
+      </c>
+      <c r="CD337">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
-    <row r="338" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -73431,8 +74128,18 @@
       <c r="CA338">
         <v>573.67032487844199</v>
       </c>
+      <c r="CB338">
+        <v>24.52</v>
+      </c>
+      <c r="CC338">
+        <v>28.92</v>
+      </c>
+      <c r="CD338">
+        <f t="shared" si="1"/>
+        <v>26.72</v>
+      </c>
     </row>
-    <row r="339" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -73619,8 +74326,18 @@
       <c r="CA339">
         <v>560.96061179772107</v>
       </c>
+      <c r="CB339">
+        <v>25.54</v>
+      </c>
+      <c r="CC339">
+        <v>28.87</v>
+      </c>
+      <c r="CD339">
+        <f t="shared" si="1"/>
+        <v>27.204999999999998</v>
+      </c>
     </row>
-    <row r="340" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -73807,8 +74524,18 @@
       <c r="CA340">
         <v>493.7601675681326</v>
       </c>
+      <c r="CB340">
+        <v>24.9</v>
+      </c>
+      <c r="CC340">
+        <v>29.19</v>
+      </c>
+      <c r="CD340">
+        <f t="shared" si="1"/>
+        <v>27.045000000000002</v>
+      </c>
     </row>
-    <row r="341" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -73998,8 +74725,18 @@
       <c r="CA341">
         <v>262.11141752057978</v>
       </c>
+      <c r="CB341">
+        <v>26.12</v>
+      </c>
+      <c r="CC341">
+        <v>30.56</v>
+      </c>
+      <c r="CD341">
+        <f t="shared" si="1"/>
+        <v>28.34</v>
+      </c>
     </row>
-    <row r="342" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -74189,8 +74926,18 @@
       <c r="CA342">
         <v>252.94563729337281</v>
       </c>
+      <c r="CB342">
+        <v>26.11</v>
+      </c>
+      <c r="CC342">
+        <v>31.95</v>
+      </c>
+      <c r="CD342">
+        <f t="shared" si="1"/>
+        <v>29.03</v>
+      </c>
     </row>
-    <row r="343" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -74380,8 +75127,18 @@
       <c r="CA343">
         <v>279.98541380051171</v>
       </c>
+      <c r="CB343">
+        <v>27.18</v>
+      </c>
+      <c r="CC343">
+        <v>32.65</v>
+      </c>
+      <c r="CD343">
+        <f t="shared" si="1"/>
+        <v>29.914999999999999</v>
+      </c>
     </row>
-    <row r="344" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -74571,8 +75328,18 @@
       <c r="CA344">
         <v>268.34223297673998</v>
       </c>
+      <c r="CB344">
+        <v>26.35</v>
+      </c>
+      <c r="CC344">
+        <v>28.27</v>
+      </c>
+      <c r="CD344">
+        <f t="shared" si="1"/>
+        <v>27.310000000000002</v>
+      </c>
     </row>
-    <row r="345" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -74762,8 +75529,18 @@
       <c r="CA345">
         <v>244.59979553880379</v>
       </c>
+      <c r="CB345">
+        <v>26.57</v>
+      </c>
+      <c r="CC345">
+        <v>31.29</v>
+      </c>
+      <c r="CD345">
+        <f t="shared" si="1"/>
+        <v>28.93</v>
+      </c>
     </row>
-    <row r="346" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -74950,8 +75727,18 @@
       <c r="CA346">
         <v>617.36397317429567</v>
       </c>
+      <c r="CB346">
+        <v>18.57</v>
+      </c>
+      <c r="CC346">
+        <v>20.91</v>
+      </c>
+      <c r="CD346">
+        <f t="shared" si="1"/>
+        <v>19.740000000000002</v>
+      </c>
     </row>
-    <row r="347" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -75138,8 +75925,18 @@
       <c r="CA347">
         <v>675.93395099194379</v>
       </c>
+      <c r="CB347">
+        <v>17.41</v>
+      </c>
+      <c r="CC347">
+        <v>19.8</v>
+      </c>
+      <c r="CD347">
+        <f t="shared" si="1"/>
+        <v>18.605</v>
+      </c>
     </row>
-    <row r="348" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -75326,8 +76123,18 @@
       <c r="CA348">
         <v>732.72304440973448</v>
       </c>
+      <c r="CB348">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="CC348">
+        <v>21.8</v>
+      </c>
+      <c r="CD348">
+        <f t="shared" si="1"/>
+        <v>18.995000000000001</v>
+      </c>
     </row>
-    <row r="349" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -75514,8 +76321,18 @@
       <c r="CA349">
         <v>683.77766141076927</v>
       </c>
+      <c r="CB349">
+        <v>18.16</v>
+      </c>
+      <c r="CC349">
+        <v>21.1</v>
+      </c>
+      <c r="CD349">
+        <f t="shared" si="1"/>
+        <v>19.630000000000003</v>
+      </c>
     </row>
-    <row r="350" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -75702,8 +76519,18 @@
       <c r="CA350">
         <v>651.16333267810342</v>
       </c>
+      <c r="CB350">
+        <v>16.82</v>
+      </c>
+      <c r="CC350">
+        <v>20.82</v>
+      </c>
+      <c r="CD350">
+        <f t="shared" si="1"/>
+        <v>18.82</v>
+      </c>
     </row>
-    <row r="351" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -75893,8 +76720,18 @@
       <c r="CA351">
         <v>220.20208177438869</v>
       </c>
+      <c r="CB351">
+        <v>17.55</v>
+      </c>
+      <c r="CC351">
+        <v>21.48</v>
+      </c>
+      <c r="CD351">
+        <f t="shared" si="1"/>
+        <v>19.515000000000001</v>
+      </c>
     </row>
-    <row r="352" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -76084,8 +76921,18 @@
       <c r="CA352">
         <v>199.39256042757091</v>
       </c>
+      <c r="CB352">
+        <v>18.98</v>
+      </c>
+      <c r="CC352">
+        <v>20.7</v>
+      </c>
+      <c r="CD352">
+        <f t="shared" si="1"/>
+        <v>19.84</v>
+      </c>
     </row>
-    <row r="353" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -76275,8 +77122,18 @@
       <c r="CA353">
         <v>173.93047619362051</v>
       </c>
+      <c r="CB353">
+        <v>18.16</v>
+      </c>
+      <c r="CC353">
+        <v>21.16</v>
+      </c>
+      <c r="CD353">
+        <f t="shared" si="1"/>
+        <v>19.66</v>
+      </c>
     </row>
-    <row r="354" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -76466,8 +77323,18 @@
       <c r="CA354">
         <v>123.756835227271</v>
       </c>
+      <c r="CB354">
+        <v>16.78</v>
+      </c>
+      <c r="CC354">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="CD354">
+        <f t="shared" si="1"/>
+        <v>18.565000000000001</v>
+      </c>
     </row>
-    <row r="355" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -76657,8 +77524,18 @@
       <c r="CA355">
         <v>231.27496370117299</v>
       </c>
+      <c r="CB355">
+        <v>17.2</v>
+      </c>
+      <c r="CC355">
+        <v>19.13</v>
+      </c>
+      <c r="CD355">
+        <f t="shared" si="1"/>
+        <v>18.164999999999999</v>
+      </c>
     </row>
-    <row r="356" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -76845,8 +77722,18 @@
       <c r="CA356">
         <v>914.04230258304028</v>
       </c>
+      <c r="CB356">
+        <v>20.45</v>
+      </c>
+      <c r="CC356">
+        <v>27</v>
+      </c>
+      <c r="CD356">
+        <f t="shared" si="1"/>
+        <v>23.725000000000001</v>
+      </c>
     </row>
-    <row r="357" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -77033,8 +77920,18 @@
       <c r="CA357">
         <v>1213.5749447289249</v>
       </c>
+      <c r="CB357">
+        <v>20.22</v>
+      </c>
+      <c r="CC357">
+        <v>26.35</v>
+      </c>
+      <c r="CD357">
+        <f t="shared" si="1"/>
+        <v>23.285</v>
+      </c>
     </row>
-    <row r="358" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -77221,8 +78118,18 @@
       <c r="CA358">
         <v>613.01285193027525</v>
       </c>
+      <c r="CB358">
+        <v>20.61</v>
+      </c>
+      <c r="CC358">
+        <v>25.1</v>
+      </c>
+      <c r="CD358">
+        <f t="shared" si="1"/>
+        <v>22.855</v>
+      </c>
     </row>
-    <row r="359" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -77409,8 +78316,18 @@
       <c r="CA359">
         <v>437.82247752403418</v>
       </c>
+      <c r="CB359">
+        <v>21.01</v>
+      </c>
+      <c r="CC359">
+        <v>26.13</v>
+      </c>
+      <c r="CD359">
+        <f t="shared" si="1"/>
+        <v>23.57</v>
+      </c>
     </row>
-    <row r="360" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -77597,8 +78514,18 @@
       <c r="CA360">
         <v>923.39312416569453</v>
       </c>
+      <c r="CB360">
+        <v>20.29</v>
+      </c>
+      <c r="CC360">
+        <v>24.64</v>
+      </c>
+      <c r="CD360">
+        <f t="shared" si="1"/>
+        <v>22.465</v>
+      </c>
     </row>
-    <row r="361" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -77789,7 +78716,7 @@
         <v>72.144443437621248</v>
       </c>
     </row>
-    <row r="362" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -77980,7 +78907,7 @@
         <v>74.71666953890508</v>
       </c>
     </row>
-    <row r="363" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -78171,7 +79098,7 @@
         <v>62.720056859920078</v>
       </c>
     </row>
-    <row r="364" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -78362,7 +79289,7 @@
         <v>68.831170614163497</v>
       </c>
     </row>
-    <row r="365" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -78553,7 +79480,7 @@
         <v>64.102054818566103</v>
       </c>
     </row>
-    <row r="366" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -78741,7 +79668,7 @@
         <v>511.62098831627969</v>
       </c>
     </row>
-    <row r="367" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -78929,7 +79856,7 @@
         <v>528.88868877453206</v>
       </c>
     </row>
-    <row r="368" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -79117,7 +80044,7 @@
         <v>584.76730967829963</v>
       </c>
     </row>
-    <row r="369" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -79305,7 +80232,7 @@
         <v>608.52600893735632</v>
       </c>
     </row>
-    <row r="370" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -79493,7 +80420,7 @@
         <v>560.05375618505877</v>
       </c>
     </row>
-    <row r="371" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -79683,8 +80610,17 @@
       <c r="CA371">
         <v>300.22111822147241</v>
       </c>
+      <c r="CB371">
+        <v>24.01</v>
+      </c>
+      <c r="CC371">
+        <v>25.99</v>
+      </c>
+      <c r="CD371">
+        <v>25</v>
+      </c>
     </row>
-    <row r="372" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -79874,8 +80810,17 @@
       <c r="CA372">
         <v>282.9002270117681</v>
       </c>
+      <c r="CB372">
+        <v>24.01</v>
+      </c>
+      <c r="CC372">
+        <v>25.99</v>
+      </c>
+      <c r="CD372">
+        <v>25</v>
+      </c>
     </row>
-    <row r="373" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -80065,8 +81010,17 @@
       <c r="CA373">
         <v>297.22554924847009</v>
       </c>
+      <c r="CB373">
+        <v>24.01</v>
+      </c>
+      <c r="CC373">
+        <v>25.99</v>
+      </c>
+      <c r="CD373">
+        <v>25</v>
+      </c>
     </row>
-    <row r="374" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -80256,8 +81210,17 @@
       <c r="CA374">
         <v>304.21170015689319</v>
       </c>
+      <c r="CB374">
+        <v>24.01</v>
+      </c>
+      <c r="CC374">
+        <v>25.99</v>
+      </c>
+      <c r="CD374">
+        <v>25</v>
+      </c>
     </row>
-    <row r="375" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -80447,8 +81410,17 @@
       <c r="CA375">
         <v>310.71660477758542</v>
       </c>
+      <c r="CB375">
+        <v>24.01</v>
+      </c>
+      <c r="CC375">
+        <v>25.99</v>
+      </c>
+      <c r="CD375">
+        <v>25</v>
+      </c>
     </row>
-    <row r="376" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -80635,8 +81607,17 @@
       <c r="CA376">
         <v>308.96933321742159</v>
       </c>
+      <c r="CB376">
+        <v>17.5</v>
+      </c>
+      <c r="CC376">
+        <v>20.46</v>
+      </c>
+      <c r="CD376">
+        <v>18.98</v>
+      </c>
     </row>
-    <row r="377" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -80823,8 +81804,17 @@
       <c r="CA377">
         <v>306.84162492206218</v>
       </c>
+      <c r="CB377">
+        <v>17.5</v>
+      </c>
+      <c r="CC377">
+        <v>20.46</v>
+      </c>
+      <c r="CD377">
+        <v>18.98</v>
+      </c>
     </row>
-    <row r="378" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -81011,8 +82001,17 @@
       <c r="CA378">
         <v>451.49734959251691</v>
       </c>
+      <c r="CB378">
+        <v>17.5</v>
+      </c>
+      <c r="CC378">
+        <v>20.46</v>
+      </c>
+      <c r="CD378">
+        <v>18.98</v>
+      </c>
     </row>
-    <row r="379" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -81199,8 +82198,17 @@
       <c r="CA379">
         <v>450.73814696790402</v>
       </c>
+      <c r="CB379">
+        <v>17.5</v>
+      </c>
+      <c r="CC379">
+        <v>20.46</v>
+      </c>
+      <c r="CD379">
+        <v>18.98</v>
+      </c>
     </row>
-    <row r="380" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -81387,8 +82395,17 @@
       <c r="CA380">
         <v>475.22572727404167</v>
       </c>
+      <c r="CB380">
+        <v>17.5</v>
+      </c>
+      <c r="CC380">
+        <v>20.46</v>
+      </c>
+      <c r="CD380">
+        <v>18.98</v>
+      </c>
     </row>
-    <row r="381" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -81578,8 +82595,17 @@
       <c r="CA381">
         <v>257.1898132626643</v>
       </c>
+      <c r="CB381">
+        <v>17.21</v>
+      </c>
+      <c r="CC381">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="CD381">
+        <v>18.325000000000003</v>
+      </c>
     </row>
-    <row r="382" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -81769,8 +82795,17 @@
       <c r="CA382">
         <v>196.8479452968395</v>
       </c>
+      <c r="CB382">
+        <v>17.21</v>
+      </c>
+      <c r="CC382">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="CD382">
+        <v>18.325000000000003</v>
+      </c>
     </row>
-    <row r="383" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -81960,8 +82995,17 @@
       <c r="CA383">
         <v>157.79934028210889</v>
       </c>
+      <c r="CB383">
+        <v>17.21</v>
+      </c>
+      <c r="CC383">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="CD383">
+        <v>18.325000000000003</v>
+      </c>
     </row>
-    <row r="384" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -82151,8 +83195,17 @@
       <c r="CA384">
         <v>182.7950191436216</v>
       </c>
+      <c r="CB384">
+        <v>17.21</v>
+      </c>
+      <c r="CC384">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="CD384">
+        <v>18.325000000000003</v>
+      </c>
     </row>
-    <row r="385" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -82342,8 +83395,17 @@
       <c r="CA385">
         <v>219.29749399429971</v>
       </c>
+      <c r="CB385">
+        <v>17.21</v>
+      </c>
+      <c r="CC385">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="CD385">
+        <v>18.325000000000003</v>
+      </c>
     </row>
-    <row r="386" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -82534,7 +83596,7 @@
         <v>280.28300294765859</v>
       </c>
     </row>
-    <row r="387" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -82725,7 +83787,7 @@
         <v>222.44653006607359</v>
       </c>
     </row>
-    <row r="388" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -82916,7 +83978,7 @@
         <v>213.76958265912981</v>
       </c>
     </row>
-    <row r="389" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -83107,7 +84169,7 @@
         <v>208.58286754296839</v>
       </c>
     </row>
-    <row r="390" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -83298,7 +84360,7 @@
         <v>205.49120449588281</v>
       </c>
     </row>
-    <row r="391" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -83488,8 +84550,17 @@
       <c r="CA391">
         <v>160.47892094167671</v>
       </c>
+      <c r="CB391">
+        <v>21.56</v>
+      </c>
+      <c r="CC391">
+        <v>23.36</v>
+      </c>
+      <c r="CD391">
+        <v>22.46</v>
+      </c>
     </row>
-    <row r="392" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -83679,8 +84750,17 @@
       <c r="CA392">
         <v>123.9910846266671</v>
       </c>
+      <c r="CB392">
+        <v>21.56</v>
+      </c>
+      <c r="CC392">
+        <v>23.36</v>
+      </c>
+      <c r="CD392">
+        <v>22.46</v>
+      </c>
     </row>
-    <row r="393" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -83870,8 +84950,17 @@
       <c r="CA393">
         <v>133.299844792567</v>
       </c>
+      <c r="CB393">
+        <v>21.56</v>
+      </c>
+      <c r="CC393">
+        <v>23.36</v>
+      </c>
+      <c r="CD393">
+        <v>22.46</v>
+      </c>
     </row>
-    <row r="394" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -84061,8 +85150,17 @@
       <c r="CA394">
         <v>149.427958417024</v>
       </c>
+      <c r="CB394">
+        <v>21.56</v>
+      </c>
+      <c r="CC394">
+        <v>23.36</v>
+      </c>
+      <c r="CD394">
+        <v>22.46</v>
+      </c>
     </row>
-    <row r="395" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -84252,8 +85350,17 @@
       <c r="CA395">
         <v>117.96033975141199</v>
       </c>
+      <c r="CB395">
+        <v>21.56</v>
+      </c>
+      <c r="CC395">
+        <v>23.36</v>
+      </c>
+      <c r="CD395">
+        <v>22.46</v>
+      </c>
     </row>
-    <row r="396" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -84444,7 +85551,7 @@
         <v>247.33905843642239</v>
       </c>
     </row>
-    <row r="397" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -84635,7 +85742,7 @@
         <v>287.02262699829771</v>
       </c>
     </row>
-    <row r="398" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -84826,7 +85933,7 @@
         <v>272.88947508843751</v>
       </c>
     </row>
-    <row r="399" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -85017,7 +86124,7 @@
         <v>221.47374266842459</v>
       </c>
     </row>
-    <row r="400" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -85208,7 +86315,7 @@
         <v>262.36983175387883</v>
       </c>
     </row>
-    <row r="401" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -85399,7 +86506,7 @@
         <v>211.05110279209339</v>
       </c>
     </row>
-    <row r="402" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -85590,7 +86697,7 @@
         <v>182.61194155473549</v>
       </c>
     </row>
-    <row r="403" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -85781,7 +86888,7 @@
         <v>178.5030410287786</v>
       </c>
     </row>
-    <row r="404" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -85972,7 +87079,7 @@
         <v>163.49969776507939</v>
       </c>
     </row>
-    <row r="405" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -86163,7 +87270,7 @@
         <v>241.6922365999603</v>
       </c>
     </row>
-    <row r="406" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -86353,8 +87460,17 @@
       <c r="CA406">
         <v>200.45523682291599</v>
       </c>
+      <c r="CB406">
+        <v>29.38</v>
+      </c>
+      <c r="CC406">
+        <v>32.01</v>
+      </c>
+      <c r="CD406">
+        <v>30.695</v>
+      </c>
     </row>
-    <row r="407" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -86544,8 +87660,17 @@
       <c r="CA407">
         <v>192.4338469110989</v>
       </c>
+      <c r="CB407">
+        <v>29.38</v>
+      </c>
+      <c r="CC407">
+        <v>32.01</v>
+      </c>
+      <c r="CD407">
+        <v>30.695</v>
+      </c>
     </row>
-    <row r="408" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -86735,8 +87860,17 @@
       <c r="CA408">
         <v>172.30901077368841</v>
       </c>
+      <c r="CB408">
+        <v>29.38</v>
+      </c>
+      <c r="CC408">
+        <v>32.01</v>
+      </c>
+      <c r="CD408">
+        <v>30.695</v>
+      </c>
     </row>
-    <row r="409" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -86926,8 +88060,17 @@
       <c r="CA409">
         <v>159.13379276642439</v>
       </c>
+      <c r="CB409">
+        <v>29.38</v>
+      </c>
+      <c r="CC409">
+        <v>32.01</v>
+      </c>
+      <c r="CD409">
+        <v>30.695</v>
+      </c>
     </row>
-    <row r="410" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -87117,8 +88260,17 @@
       <c r="CA410">
         <v>236.38011337154921</v>
       </c>
+      <c r="CB410">
+        <v>29.38</v>
+      </c>
+      <c r="CC410">
+        <v>32.01</v>
+      </c>
+      <c r="CD410">
+        <v>30.695</v>
+      </c>
     </row>
-    <row r="411" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -87308,8 +88460,17 @@
       <c r="CA411">
         <v>158.75664056211741</v>
       </c>
+      <c r="CB411">
+        <v>32.71</v>
+      </c>
+      <c r="CC411">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="CD411">
+        <v>32.504999999999995</v>
+      </c>
     </row>
-    <row r="412" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -87499,8 +88660,17 @@
       <c r="CA412">
         <v>183.48941543026879</v>
       </c>
+      <c r="CB412">
+        <v>32.71</v>
+      </c>
+      <c r="CC412">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="CD412">
+        <v>32.504999999999995</v>
+      </c>
     </row>
-    <row r="413" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -87690,8 +88860,17 @@
       <c r="CA413">
         <v>156.36523348644189</v>
       </c>
+      <c r="CB413">
+        <v>32.71</v>
+      </c>
+      <c r="CC413">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="CD413">
+        <v>32.504999999999995</v>
+      </c>
     </row>
-    <row r="414" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -87881,8 +89060,17 @@
       <c r="CA414">
         <v>151.058755479979</v>
       </c>
+      <c r="CB414">
+        <v>32.71</v>
+      </c>
+      <c r="CC414">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="CD414">
+        <v>32.504999999999995</v>
+      </c>
     </row>
-    <row r="415" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -88072,8 +89260,17 @@
       <c r="CA415">
         <v>143.620798505799</v>
       </c>
+      <c r="CB415">
+        <v>32.71</v>
+      </c>
+      <c r="CC415">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="CD415">
+        <v>32.504999999999995</v>
+      </c>
     </row>
-    <row r="416" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -88264,7 +89461,7 @@
         <v>174.07487240349431</v>
       </c>
     </row>
-    <row r="417" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -88455,7 +89652,7 @@
         <v>205.1809903469229</v>
       </c>
     </row>
-    <row r="418" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -88646,7 +89843,7 @@
         <v>196.5452780100309</v>
       </c>
     </row>
-    <row r="419" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -88837,7 +90034,7 @@
         <v>171.82233179572719</v>
       </c>
     </row>
-    <row r="420" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -89028,7 +90225,7 @@
         <v>232.85281178681231</v>
       </c>
     </row>
-    <row r="421" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -89218,8 +90415,17 @@
       <c r="CA421">
         <v>231.3959276825704</v>
       </c>
+      <c r="CB421">
+        <v>31.88</v>
+      </c>
+      <c r="CC421">
+        <v>33.58</v>
+      </c>
+      <c r="CD421">
+        <v>32.729999999999997</v>
+      </c>
     </row>
-    <row r="422" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -89409,8 +90615,17 @@
       <c r="CA422">
         <v>217.18159202329289</v>
       </c>
+      <c r="CB422">
+        <v>31.88</v>
+      </c>
+      <c r="CC422">
+        <v>33.58</v>
+      </c>
+      <c r="CD422">
+        <v>32.729999999999997</v>
+      </c>
     </row>
-    <row r="423" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -89600,8 +90815,17 @@
       <c r="CA423">
         <v>140.6952906236165</v>
       </c>
+      <c r="CB423">
+        <v>31.88</v>
+      </c>
+      <c r="CC423">
+        <v>33.58</v>
+      </c>
+      <c r="CD423">
+        <v>32.729999999999997</v>
+      </c>
     </row>
-    <row r="424" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -89791,8 +91015,17 @@
       <c r="CA424">
         <v>151.26774141320129</v>
       </c>
+      <c r="CB424">
+        <v>31.88</v>
+      </c>
+      <c r="CC424">
+        <v>33.58</v>
+      </c>
+      <c r="CD424">
+        <v>32.729999999999997</v>
+      </c>
     </row>
-    <row r="425" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -89982,8 +91215,17 @@
       <c r="CA425">
         <v>179.94924778685069</v>
       </c>
+      <c r="CB425">
+        <v>31.88</v>
+      </c>
+      <c r="CC425">
+        <v>33.58</v>
+      </c>
+      <c r="CD425">
+        <v>32.729999999999997</v>
+      </c>
     </row>
-    <row r="426" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -90174,7 +91416,7 @@
         <v>175.87548898268</v>
       </c>
     </row>
-    <row r="427" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -90365,7 +91607,7 @@
         <v>147.50134760814441</v>
       </c>
     </row>
-    <row r="428" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -90556,7 +91798,7 @@
         <v>169.53076303796391</v>
       </c>
     </row>
-    <row r="429" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -90747,7 +91989,7 @@
         <v>152.77643486792391</v>
       </c>
     </row>
-    <row r="430" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -90938,7 +92180,7 @@
         <v>203.86824986424011</v>
       </c>
     </row>
-    <row r="431" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -91128,8 +92370,17 @@
       <c r="CA431">
         <v>301.90658448858773</v>
       </c>
+      <c r="CB431">
+        <v>25.66</v>
+      </c>
+      <c r="CC431">
+        <v>26.12</v>
+      </c>
+      <c r="CD431">
+        <v>25.89</v>
+      </c>
     </row>
-    <row r="432" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -91319,8 +92570,17 @@
       <c r="CA432">
         <v>205.05409605755321</v>
       </c>
+      <c r="CB432">
+        <v>25.66</v>
+      </c>
+      <c r="CC432">
+        <v>26.12</v>
+      </c>
+      <c r="CD432">
+        <v>25.89</v>
+      </c>
     </row>
-    <row r="433" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -91510,8 +92770,17 @@
       <c r="CA433">
         <v>216.87638246654029</v>
       </c>
+      <c r="CB433">
+        <v>25.66</v>
+      </c>
+      <c r="CC433">
+        <v>26.12</v>
+      </c>
+      <c r="CD433">
+        <v>25.89</v>
+      </c>
     </row>
-    <row r="434" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -91701,8 +92970,17 @@
       <c r="CA434">
         <v>211.53670504201449</v>
       </c>
+      <c r="CB434">
+        <v>25.66</v>
+      </c>
+      <c r="CC434">
+        <v>26.12</v>
+      </c>
+      <c r="CD434">
+        <v>25.89</v>
+      </c>
     </row>
-    <row r="435" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -91892,8 +93170,17 @@
       <c r="CA435">
         <v>159.54655771620591</v>
       </c>
+      <c r="CB435">
+        <v>25.66</v>
+      </c>
+      <c r="CC435">
+        <v>26.12</v>
+      </c>
+      <c r="CD435">
+        <v>25.89</v>
+      </c>
     </row>
-    <row r="436" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -92081,7 +93368,7 @@
         <v>222.9771719354753</v>
       </c>
     </row>
-    <row r="437" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -92269,7 +93556,7 @@
         <v>283.05241329246519</v>
       </c>
     </row>
-    <row r="438" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -92457,7 +93744,7 @@
         <v>207.74812114931549</v>
       </c>
     </row>
-    <row r="439" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -92645,7 +93932,7 @@
         <v>213.17388081513349</v>
       </c>
     </row>
-    <row r="440" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -92833,7 +94120,7 @@
         <v>324.35952144477187</v>
       </c>
     </row>
-    <row r="441" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -93023,8 +94310,17 @@
       <c r="CA441">
         <v>152.88832498100561</v>
       </c>
+      <c r="CB441">
+        <v>22.78</v>
+      </c>
+      <c r="CC441">
+        <v>23.6</v>
+      </c>
+      <c r="CD441">
+        <v>23.19</v>
+      </c>
     </row>
-    <row r="442" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -93214,8 +94510,17 @@
       <c r="CA442">
         <v>122.50317260246899</v>
       </c>
+      <c r="CB442">
+        <v>22.78</v>
+      </c>
+      <c r="CC442">
+        <v>23.6</v>
+      </c>
+      <c r="CD442">
+        <v>23.19</v>
+      </c>
     </row>
-    <row r="443" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -93405,8 +94710,17 @@
       <c r="CA443">
         <v>178.19405020618751</v>
       </c>
+      <c r="CB443">
+        <v>22.78</v>
+      </c>
+      <c r="CC443">
+        <v>23.6</v>
+      </c>
+      <c r="CD443">
+        <v>23.19</v>
+      </c>
     </row>
-    <row r="444" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -93596,8 +94910,17 @@
       <c r="CA444">
         <v>144.00370330139319</v>
       </c>
+      <c r="CB444">
+        <v>22.78</v>
+      </c>
+      <c r="CC444">
+        <v>23.6</v>
+      </c>
+      <c r="CD444">
+        <v>23.19</v>
+      </c>
     </row>
-    <row r="445" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>443</v>
       </c>
@@ -93787,8 +95110,17 @@
       <c r="CA445">
         <v>110.51502168721839</v>
       </c>
+      <c r="CB445">
+        <v>22.78</v>
+      </c>
+      <c r="CC445">
+        <v>23.6</v>
+      </c>
+      <c r="CD445">
+        <v>23.19</v>
+      </c>
     </row>
-    <row r="446" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -93976,7 +95308,7 @@
         <v>203.14021668186521</v>
       </c>
     </row>
-    <row r="447" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>445</v>
       </c>
@@ -94164,7 +95496,7 @@
         <v>133.86626189599701</v>
       </c>
     </row>
-    <row r="448" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>446</v>
       </c>
@@ -94352,7 +95684,7 @@
         <v>153.01093365552009</v>
       </c>
     </row>
-    <row r="449" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>447</v>
       </c>
@@ -94540,7 +95872,7 @@
         <v>129.64247423976619</v>
       </c>
     </row>
-    <row r="450" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>448</v>
       </c>
@@ -94728,7 +96060,7 @@
         <v>174.33378436488329</v>
       </c>
     </row>
-    <row r="451" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>449</v>
       </c>
@@ -94919,7 +96251,7 @@
         <v>146.8090707349829</v>
       </c>
     </row>
-    <row r="452" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>450</v>
       </c>
@@ -95110,7 +96442,7 @@
         <v>122.7973806083892</v>
       </c>
     </row>
-    <row r="453" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -95301,7 +96633,7 @@
         <v>178.1544914993483</v>
       </c>
     </row>
-    <row r="454" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>452</v>
       </c>
@@ -95492,7 +96824,7 @@
         <v>182.22797123150119</v>
       </c>
     </row>
-    <row r="455" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>453</v>
       </c>
@@ -95683,7 +97015,7 @@
         <v>171.89379872976949</v>
       </c>
     </row>
-    <row r="456" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>454</v>
       </c>
@@ -95870,8 +97202,17 @@
       <c r="CA456">
         <v>394.74718793507918</v>
       </c>
+      <c r="CB456">
+        <v>25.5</v>
+      </c>
+      <c r="CC456">
+        <v>29.15</v>
+      </c>
+      <c r="CD456">
+        <v>27.324999999999999</v>
+      </c>
     </row>
-    <row r="457" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>455</v>
       </c>
@@ -96058,8 +97399,17 @@
       <c r="CA457">
         <v>382.99560236385878</v>
       </c>
+      <c r="CB457">
+        <v>25.5</v>
+      </c>
+      <c r="CC457">
+        <v>29.15</v>
+      </c>
+      <c r="CD457">
+        <v>27.324999999999999</v>
+      </c>
     </row>
-    <row r="458" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>456</v>
       </c>
@@ -96246,8 +97596,17 @@
       <c r="CA458">
         <v>376.91035513177218</v>
       </c>
+      <c r="CB458">
+        <v>25.5</v>
+      </c>
+      <c r="CC458">
+        <v>29.15</v>
+      </c>
+      <c r="CD458">
+        <v>27.324999999999999</v>
+      </c>
     </row>
-    <row r="459" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>457</v>
       </c>
@@ -96434,8 +97793,17 @@
       <c r="CA459">
         <v>294.96755597734591</v>
       </c>
+      <c r="CB459">
+        <v>25.5</v>
+      </c>
+      <c r="CC459">
+        <v>29.15</v>
+      </c>
+      <c r="CD459">
+        <v>27.324999999999999</v>
+      </c>
     </row>
-    <row r="460" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -96622,8 +97990,17 @@
       <c r="CA460">
         <v>421.18771985123288</v>
       </c>
+      <c r="CB460">
+        <v>25.5</v>
+      </c>
+      <c r="CC460">
+        <v>29.15</v>
+      </c>
+      <c r="CD460">
+        <v>27.324999999999999</v>
+      </c>
     </row>
-    <row r="461" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>459</v>
       </c>
@@ -96813,8 +98190,17 @@
       <c r="CA461">
         <v>312.45895081042642</v>
       </c>
+      <c r="CB461">
+        <v>21.18</v>
+      </c>
+      <c r="CC461">
+        <v>26.57</v>
+      </c>
+      <c r="CD461">
+        <v>23.875</v>
+      </c>
     </row>
-    <row r="462" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>460</v>
       </c>
@@ -97004,8 +98390,17 @@
       <c r="CA462">
         <v>352.59393734146528</v>
       </c>
+      <c r="CB462">
+        <v>21.18</v>
+      </c>
+      <c r="CC462">
+        <v>26.57</v>
+      </c>
+      <c r="CD462">
+        <v>23.875</v>
+      </c>
     </row>
-    <row r="463" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>461</v>
       </c>
@@ -97195,8 +98590,17 @@
       <c r="CA463">
         <v>287.16986297837548</v>
       </c>
+      <c r="CB463">
+        <v>21.18</v>
+      </c>
+      <c r="CC463">
+        <v>26.57</v>
+      </c>
+      <c r="CD463">
+        <v>23.875</v>
+      </c>
     </row>
-    <row r="464" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>462</v>
       </c>
@@ -97386,8 +98790,17 @@
       <c r="CA464">
         <v>301.15778355893639</v>
       </c>
+      <c r="CB464">
+        <v>21.18</v>
+      </c>
+      <c r="CC464">
+        <v>26.57</v>
+      </c>
+      <c r="CD464">
+        <v>23.875</v>
+      </c>
     </row>
-    <row r="465" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>463</v>
       </c>
@@ -97577,8 +98990,17 @@
       <c r="CA465">
         <v>331.82066142474878</v>
       </c>
+      <c r="CB465">
+        <v>21.18</v>
+      </c>
+      <c r="CC465">
+        <v>26.57</v>
+      </c>
+      <c r="CD465">
+        <v>23.875</v>
+      </c>
     </row>
-    <row r="466" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>464</v>
       </c>
@@ -97766,7 +99188,7 @@
         <v>260.41241548814787</v>
       </c>
     </row>
-    <row r="467" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>465</v>
       </c>
@@ -97954,7 +99376,7 @@
         <v>231.4914741509233</v>
       </c>
     </row>
-    <row r="468" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -98142,7 +99564,7 @@
         <v>166.43218564782589</v>
       </c>
     </row>
-    <row r="469" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>467</v>
       </c>
@@ -98330,7 +99752,7 @@
         <v>161.00656800086381</v>
       </c>
     </row>
-    <row r="470" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>468</v>
       </c>
@@ -98518,7 +99940,7 @@
         <v>269.83092047685699</v>
       </c>
     </row>
-    <row r="471" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>469</v>
       </c>
@@ -98709,7 +100131,7 @@
         <v>333.72516214884041</v>
       </c>
     </row>
-    <row r="472" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>470</v>
       </c>
@@ -98900,7 +100322,7 @@
         <v>293.72787983737732</v>
       </c>
     </row>
-    <row r="473" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>471</v>
       </c>
@@ -99091,7 +100513,7 @@
         <v>278.07448393687167</v>
       </c>
     </row>
-    <row r="474" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>472</v>
       </c>
@@ -99282,7 +100704,7 @@
         <v>308.10131016157402</v>
       </c>
     </row>
-    <row r="475" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>473</v>
       </c>
@@ -99473,7 +100895,7 @@
         <v>315.5880793586939</v>
       </c>
     </row>
-    <row r="476" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>474</v>
       </c>
@@ -99660,8 +101082,17 @@
       <c r="CA476">
         <v>335.50806576551309</v>
       </c>
+      <c r="CB476">
+        <v>25.28</v>
+      </c>
+      <c r="CC476">
+        <v>24.06</v>
+      </c>
+      <c r="CD476">
+        <v>24.67</v>
+      </c>
     </row>
-    <row r="477" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>475</v>
       </c>
@@ -99848,8 +101279,17 @@
       <c r="CA477">
         <v>323.97224297601042</v>
       </c>
+      <c r="CB477">
+        <v>25.28</v>
+      </c>
+      <c r="CC477">
+        <v>24.06</v>
+      </c>
+      <c r="CD477">
+        <v>24.67</v>
+      </c>
     </row>
-    <row r="478" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>476</v>
       </c>
@@ -100036,8 +101476,17 @@
       <c r="CA478">
         <v>315.04901015437281</v>
       </c>
+      <c r="CB478">
+        <v>25.28</v>
+      </c>
+      <c r="CC478">
+        <v>24.06</v>
+      </c>
+      <c r="CD478">
+        <v>24.67</v>
+      </c>
     </row>
-    <row r="479" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>477</v>
       </c>
@@ -100224,8 +101673,17 @@
       <c r="CA479">
         <v>317.48253994553852</v>
       </c>
+      <c r="CB479">
+        <v>25.28</v>
+      </c>
+      <c r="CC479">
+        <v>24.06</v>
+      </c>
+      <c r="CD479">
+        <v>24.67</v>
+      </c>
     </row>
-    <row r="480" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>478</v>
       </c>
@@ -100412,8 +101870,17 @@
       <c r="CA480">
         <v>392.00718426622598</v>
       </c>
+      <c r="CB480">
+        <v>25.28</v>
+      </c>
+      <c r="CC480">
+        <v>24.06</v>
+      </c>
+      <c r="CD480">
+        <v>24.67</v>
+      </c>
     </row>
-    <row r="481" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>479</v>
       </c>
@@ -100603,8 +102070,17 @@
       <c r="CA481">
         <v>336.14963125836948</v>
       </c>
+      <c r="CB481">
+        <v>26.06</v>
+      </c>
+      <c r="CC481">
+        <v>26.08</v>
+      </c>
+      <c r="CD481">
+        <v>26.07</v>
+      </c>
     </row>
-    <row r="482" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <v>480</v>
       </c>
@@ -100794,8 +102270,17 @@
       <c r="CA482">
         <v>270.77721424034331</v>
       </c>
+      <c r="CB482">
+        <v>26.06</v>
+      </c>
+      <c r="CC482">
+        <v>26.08</v>
+      </c>
+      <c r="CD482">
+        <v>26.07</v>
+      </c>
     </row>
-    <row r="483" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>481</v>
       </c>
@@ -100985,8 +102470,17 @@
       <c r="CA483">
         <v>361.79524087647872</v>
       </c>
+      <c r="CB483">
+        <v>26.06</v>
+      </c>
+      <c r="CC483">
+        <v>26.08</v>
+      </c>
+      <c r="CD483">
+        <v>26.07</v>
+      </c>
     </row>
-    <row r="484" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A484" s="1">
         <v>482</v>
       </c>
@@ -101176,8 +102670,17 @@
       <c r="CA484">
         <v>399.96961069665292</v>
       </c>
+      <c r="CB484">
+        <v>26.06</v>
+      </c>
+      <c r="CC484">
+        <v>26.08</v>
+      </c>
+      <c r="CD484">
+        <v>26.07</v>
+      </c>
     </row>
-    <row r="485" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <v>483</v>
       </c>
@@ -101366,10 +102869,20 @@
       </c>
       <c r="CA485">
         <v>345.83732493346002</v>
+      </c>
+      <c r="CB485">
+        <v>26.06</v>
+      </c>
+      <c r="CC485">
+        <v>26.08</v>
+      </c>
+      <c r="CD485">
+        <v>26.07</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>